<commit_message>
Added Void Seeders expansion data
</commit_message>
<xml_diff>
--- a/Data/Cards_and_Tokens.xlsx
+++ b/Data/Cards_and_Tokens.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saku\WebstormProjects\AlienBag\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B96E35-7E93-434B-9FA1-98042B75D6E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24F11FC-5F68-4235-8B2D-7583E6C3B6A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4185" windowWidth="15990" windowHeight="24840" xr2:uid="{E69D66DF-7E14-4EE4-A525-8A32B9516520}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{E69D66DF-7E14-4EE4-A525-8A32B9516520}"/>
   </bookViews>
   <sheets>
     <sheet name="Tokens" sheetId="1" r:id="rId1"/>
     <sheet name="Event Cards" sheetId="2" r:id="rId2"/>
     <sheet name="Intruder Attack" sheetId="3" r:id="rId3"/>
+    <sheet name="VoidSeeders Tokens" sheetId="4" r:id="rId4"/>
+    <sheet name="VoidSeeders Event Cards" sheetId="5" r:id="rId5"/>
+    <sheet name="Voidseeders Attack Cards" sheetId="6" r:id="rId6"/>
+    <sheet name="Voidseeders Panic Cards" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet5" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="226">
   <si>
     <t>ID</t>
   </si>
@@ -426,6 +431,291 @@
   </si>
   <si>
     <t>Nothing appears</t>
+  </si>
+  <si>
+    <t>~/img</t>
+  </si>
+  <si>
+    <t>Void Seeder appears. Character's insanity level determines the enemy type.</t>
+  </si>
+  <si>
+    <t>All players perform a Noise roll in order, except if their Character is already in Combat with a Void Seeder or a Lair.</t>
+  </si>
+  <si>
+    <t>Void Seeder</t>
+  </si>
+  <si>
+    <t>Blue Insanity Token</t>
+  </si>
+  <si>
+    <t>Red Insanity Token</t>
+  </si>
+  <si>
+    <t>Yellow Insanity Token</t>
+  </si>
+  <si>
+    <t>Green Insanity Token</t>
+  </si>
+  <si>
+    <t>Purple Insanity Token</t>
+  </si>
+  <si>
+    <t>Grey Insanity Token</t>
+  </si>
+  <si>
+    <t>Blank Token</t>
+  </si>
+  <si>
+    <t>Place a noise marker in each Corridor connected to the corridor where the encounter took place. Resolve a Panic card.</t>
+  </si>
+  <si>
+    <t>Place a noise marker in each Corridor connected to the corridor where the encounter took place.</t>
+  </si>
+  <si>
+    <t>Pink Insanity Token</t>
+  </si>
+  <si>
+    <t>Player resolves a Panic card.</t>
+  </si>
+  <si>
+    <t>Nothing Happens.</t>
+  </si>
+  <si>
+    <t>Lurker</t>
+  </si>
+  <si>
+    <t>Whisperer</t>
+  </si>
+  <si>
+    <t>Stalker</t>
+  </si>
+  <si>
+    <t>Despoiler</t>
+  </si>
+  <si>
+    <t>Terror</t>
+  </si>
+  <si>
+    <t>Each Character draws cards from their Action deck until they have 5 cards in hand and then Scans all their Contamination cards. If they have at least 1 INFECTED result, increase their Insanity level to 5. Afterward, all Characters discard all cards from their hands.</t>
+  </si>
+  <si>
+    <t>Each Void Seeder not in Combat moves to a neighboring Room containing a Character, if possible. If several Rooms are eligible, it moves to the Room with the lower number. Otherwise, it does not move.</t>
+  </si>
+  <si>
+    <t>Tendrils</t>
+  </si>
+  <si>
+    <t>Every Character in a Room with Technical Corridors increses their Insanity Level.</t>
+  </si>
+  <si>
+    <t>Computer System Failure</t>
+  </si>
+  <si>
+    <t>If there is a Malfunction marker in any Room with a Computer, place a Malfunction marker in each other Room with a Computer. Remove this card from the game and reshuffle the Event deck.</t>
+  </si>
+  <si>
+    <t>Monophobia</t>
+  </si>
+  <si>
+    <t>Each Character alone in a Room and not in Combat resolves a Panic card.</t>
+  </si>
+  <si>
+    <t>Neurosis</t>
+  </si>
+  <si>
+    <t>Every Character in a Room with a Lair or in a Room neighboring a Lair draws a Panic card and resolves it.</t>
+  </si>
+  <si>
+    <t>Agoraphobia</t>
+  </si>
+  <si>
+    <t>If there is more than 1 Character in a Room, place a Despoiler in that Room. Do not Resolve a Surprise Attack. If there is more than 1 Room eligible it appears in the Room with the lower number.</t>
+  </si>
+  <si>
+    <t>Remove the Escape pod token with the lower number. Remove this card from the game and reshuffle the Event deck (including the Discard Pile.)</t>
+  </si>
+  <si>
+    <t>If there is a Malfunction marker in any Room with a Computer, place a Malfunction marker in each other Room with a Computer.</t>
+  </si>
+  <si>
+    <t>Remove the Escape pod token with the lowest number.</t>
+  </si>
+  <si>
+    <t>Fire Wave</t>
+  </si>
+  <si>
+    <t>Find the Room with the lower number containing a Fire marker. Place a Fire marker in each neighboring Room. Fire does not spread through Closed Doors of Technical Corridors.</t>
+  </si>
+  <si>
+    <t>Generator Overheat</t>
+  </si>
+  <si>
+    <t>If there is a Malfunction marker in the Generator Room, place a Fire marker in that Room. Place a Fire marker in each Room neighboring a Room with a Fire marker. Fire does not spread through Closed doors or Technical Corridors. If there is no Malfunction marker in the Generator Room, place a Malfunction marker in that Room. Remove this card from the game and reshuffle the Event deck (including discard pile).</t>
+  </si>
+  <si>
+    <t>If there is a Malfunction marker in the Generator Room, place a Fire marker in that Room. Place a Fire marker in each Room neighboring a Room with a Fire marker. Fire does not spread through Closed doors or Technical Corridors. If there is no Malfunction marker in the Generator Room, place a Malfunction marker in that Room.</t>
+  </si>
+  <si>
+    <t>Whispers</t>
+  </si>
+  <si>
+    <t>Draw another Event card, then place a Noise marker in each Corridor with the same number than the one on this new Evetn card and that is connected to a Room containing a Character. If a Corridor already contains a Noise marker, resolve and Encounter instead. Afterward discard the new Event card without resolving it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Place a noise marker in in each Corridor numbered above. If a Corridor already contains a Noise marker, resolve and Encounter instead. </t>
+  </si>
+  <si>
+    <t>Fear</t>
+  </si>
+  <si>
+    <t>Every Character whose Insanity level is higher than the number of cards in their hand is dealt a Contamination card.</t>
+  </si>
+  <si>
+    <t>Fuel Explosion</t>
+  </si>
+  <si>
+    <t>Place a Fire marker in each Engine. Remove this card from the game and reshuffle the Event deck (including discard pile).</t>
+  </si>
+  <si>
+    <t>Place a Fire marker in each Engine.</t>
+  </si>
+  <si>
+    <t>Ship AI Failure</t>
+  </si>
+  <si>
+    <t>If there are at least 2 Malfunction markers in a Room with a Computer, start Self-Destruct sequence. Otherwise, place a Malfunction marker in the Room with the lowest number containing a Computer.</t>
+  </si>
+  <si>
+    <t>Any Character in the Room who has suffered at least 1 Serious Wound dies. All other Characters in this Room suffer 1 Serious Wound and increase their insanity level.</t>
+  </si>
+  <si>
+    <t>The Character suffers 1 Light Wound and gets a Contamination card.</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>Take the Void Seeder miniature corresponding to the symbol of the Character's Insanity level on the Insanity track and place it in the Room. This Void Seeder doesn't perform a Surprise Attack nor attacks during the current Attack step.</t>
+  </si>
+  <si>
+    <t>The Character suffers 1 Serious Wound. Draw and resolve a Panic card.</t>
+  </si>
+  <si>
+    <t>Braineating</t>
+  </si>
+  <si>
+    <t>If player has at least 1 Serious Wound, they die. Otherwise, they suffer 2 Serious Wounds.</t>
+  </si>
+  <si>
+    <t>If the Character has at leat 2 Serious Wounds, they die. Otherwise, they suffer 1 Serious Wound.</t>
+  </si>
+  <si>
+    <t>The Character gets a Contamination card. Draw and resolve a Panic card.</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>PanicName</t>
+  </si>
+  <si>
+    <t>CardText</t>
+  </si>
+  <si>
+    <t>AppText</t>
+  </si>
+  <si>
+    <t>InsanityLevel</t>
+  </si>
+  <si>
+    <t>SpecialRuleId</t>
+  </si>
+  <si>
+    <t>Desctructive Outburst</t>
+  </si>
+  <si>
+    <t>Place a Malfunction marker in the Room you are in, if there is none.</t>
+  </si>
+  <si>
+    <t>Defeatism</t>
+  </si>
+  <si>
+    <t>Increase the Insanity level of every Character in the Room you are in (including you) by 1.</t>
+  </si>
+  <si>
+    <t>Blind Escape</t>
+  </si>
+  <si>
+    <t>Draw an Event card and move your Character through indicated corridor</t>
+  </si>
+  <si>
+    <t>Desctruction</t>
+  </si>
+  <si>
+    <t>Discard a Heavy Item from your hand, if possible (not a Heavy Object)</t>
+  </si>
+  <si>
+    <t>Insane Courage</t>
+  </si>
+  <si>
+    <t>Move your Character to a neighboring Room with a Void Seeder.</t>
+  </si>
+  <si>
+    <t>Sabotage</t>
+  </si>
+  <si>
+    <t>Set the item counter to 0 in the Room you are in.</t>
+  </si>
+  <si>
+    <t>Self-Mutilation</t>
+  </si>
+  <si>
+    <t>Deal 2 Light Wounds to yourself.</t>
+  </si>
+  <si>
+    <t>Heart Attack</t>
+  </si>
+  <si>
+    <t>Your Character dies.</t>
+  </si>
+  <si>
+    <t>Bloodlust</t>
+  </si>
+  <si>
+    <t>Deal 1 Serious Wound to every other Character in the Room you are in. If you are alone, deal 1 Serious Wound to yourself.</t>
+  </si>
+  <si>
+    <t>Demotivation</t>
+  </si>
+  <si>
+    <t>Each Character in the Room you are in (including yourself) discards 1 Action card from their hand. Increase your Insanity lever by 1.</t>
+  </si>
+  <si>
+    <t>Ripping of the Bandages</t>
+  </si>
+  <si>
+    <t>Deal 1 Light Wound to yourself and undress 1 Serious Wound.</t>
+  </si>
+  <si>
+    <t>Hopelessness</t>
+  </si>
+  <si>
+    <t>Draw 3 cards from your Action deck and remove one of them from the game. Discard the rest.</t>
+  </si>
+  <si>
+    <t>Hallucinations</t>
+  </si>
+  <si>
+    <t>Discard all Ammo markers from one of your weapons.</t>
+  </si>
+  <si>
+    <t>Pyromaniac</t>
+  </si>
+  <si>
+    <t>Place a Fire marker in the Room you are in, if there is none.</t>
   </si>
 </sst>
 </file>
@@ -788,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{654AAEDF-C7D1-4F87-A8A6-CACAA664CB2C}">
   <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U3" sqref="U3:V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,8 +1898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B63CAED-B215-44CA-8867-65B47B1CA3A3}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2623,8 +2913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B58D991-A21A-4C38-B7BF-882E7A05689A}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3125,4 +3415,2390 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75492530-C307-4ABE-A721-90BABCA61327}">
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="34" customWidth="1"/>
+    <col min="6" max="6" width="65.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="46" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>134</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>136</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>137</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>138</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H23" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H24" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>140</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H25" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26">
+        <v>9</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAE4B4F2-93DF-469E-87F5-6372484E413F}">
+  <dimension ref="A1:O21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="55.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="54.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="L2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="L3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="L4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="L5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="L6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="L7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="L8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="L9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="L10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="L11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="2">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="L12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="120" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="L14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="2">
+        <v>3</v>
+      </c>
+      <c r="D15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="L15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="L16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="2">
+        <v>4</v>
+      </c>
+      <c r="D17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="L17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="L18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="L19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3</v>
+      </c>
+      <c r="D20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="L20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N20" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="2">
+        <v>3</v>
+      </c>
+      <c r="D21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="L21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE613A7-D59E-412E-BD43-A0C3D1ED0F5B}">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="3" customWidth="1"/>
+    <col min="2" max="4" width="39.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E3" s="3">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E4" s="3">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E5" s="3">
+        <v>6</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E6" s="3">
+        <v>4</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E10" s="3">
+        <v>4</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E13" s="3">
+        <v>5</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E14" s="3">
+        <v>4</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E15" s="3">
+        <v>3</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E16" s="3">
+        <v>2</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E18" s="3">
+        <v>5</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E19" s="3">
+        <v>4</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E20" s="3">
+        <v>2</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E21" s="3">
+        <v>2</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E14948D-5C43-4D1C-AD13-A47B8A6652B9}">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" style="3" customWidth="1"/>
+    <col min="5" max="6" width="16.85546875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E3" s="3">
+        <v>3</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E5" s="3">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E9" s="3">
+        <v>5</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E10" s="3">
+        <v>5</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E11" s="3">
+        <v>3</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E13" s="3">
+        <v>3</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E14" s="3">
+        <v>2</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E15" s="3">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="E16" s="3">
+        <v>3</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E17" s="3">
+        <v>3</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E18" s="3">
+        <v>3</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E19" s="3">
+        <v>3</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="E20" s="3">
+        <v>3</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E30861-0791-4016-9E0B-88A45FC5FB27}">
+  <dimension ref="A3:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixes to token descriptions
</commit_message>
<xml_diff>
--- a/Data/Cards_and_Tokens.xlsx
+++ b/Data/Cards_and_Tokens.xlsx
@@ -8,9 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saku\WebstormProjects\AlienBag\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24F11FC-5F68-4235-8B2D-7583E6C3B6A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BAFB65-40AA-4AE0-AC6E-92117A898A9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{E69D66DF-7E14-4EE4-A525-8A32B9516520}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="8" xr2:uid="{E69D66DF-7E14-4EE4-A525-8A32B9516520}"/>
+    <workbookView xWindow="28680" yWindow="-4185" windowWidth="15990" windowHeight="24840" activeTab="1" xr2:uid="{99D5B4DA-9CD6-4AED-9D6A-82F7E738FFC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tokens" sheetId="1" r:id="rId1"/>
@@ -21,6 +22,7 @@
     <sheet name="Voidseeders Attack Cards" sheetId="6" r:id="rId6"/>
     <sheet name="Voidseeders Panic Cards" sheetId="7" r:id="rId7"/>
     <sheet name="Sheet5" sheetId="8" r:id="rId8"/>
+    <sheet name="AfterMath Event Deck" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="250">
   <si>
     <t>ID</t>
   </si>
@@ -716,6 +718,78 @@
   </si>
   <si>
     <t>Place a Fire marker in the Room you are in, if there is none.</t>
+  </si>
+  <si>
+    <t>Place a Malfunction marker in each explorer Green Room.</t>
+  </si>
+  <si>
+    <t>[1,4,5]</t>
+  </si>
+  <si>
+    <t>Infested Supplies</t>
+  </si>
+  <si>
+    <t>All Characters In Green Rooms add a Contamination Card to their Discard Pile.</t>
+  </si>
+  <si>
+    <t>[1,2,3]</t>
+  </si>
+  <si>
+    <t>Dripping</t>
+  </si>
+  <si>
+    <t>All Characters In every Room with Technical Corridors get a Slime marker.</t>
+  </si>
+  <si>
+    <t>Slimy</t>
+  </si>
+  <si>
+    <t>Each Character with a Slime marker adds 2 Contamination cards to their Discard pile.</t>
+  </si>
+  <si>
+    <t>Royal Ceremony</t>
+  </si>
+  <si>
+    <t>If the Queen is not in play, place her in the Nest. If the Queen is already in play or if the Nest hasn't been discovered, add an additional Egg token on the Intruder board.</t>
+  </si>
+  <si>
+    <t>Eggs Hatching</t>
+  </si>
+  <si>
+    <t>Place a Larva miniature in each Room with an Egg token. Place 1 Larva miniature in the Nest. Remove all Egg tokens from the main board.</t>
+  </si>
+  <si>
+    <t>Sparks</t>
+  </si>
+  <si>
+    <t>Place a Fire Marker in each Room with a Malfunction marker.</t>
+  </si>
+  <si>
+    <t>Screeching</t>
+  </si>
+  <si>
+    <t>Place a Noise marker in each Corridor connected to every room with an Intruder</t>
+  </si>
+  <si>
+    <t>Adaptability</t>
+  </si>
+  <si>
+    <t>Discard 1 discovered Intruder Weakness</t>
+  </si>
+  <si>
+    <t>Maneuver</t>
+  </si>
+  <si>
+    <t>All Characters draw 1 less Action Card next turn.</t>
+  </si>
+  <si>
+    <t>Warbling</t>
+  </si>
+  <si>
+    <t>Place a Noise marker in each Corridor connected to an Engine Room. Roll a Combat die for each Engine in order - on a results of O or OO, switch that Engine's status . When you have switched 1 Engine status, do not roll for the  remaining Engines.</t>
+  </si>
+  <si>
+    <t>Speciel Case 5: Alert: Drawn an alert card.</t>
   </si>
 </sst>
 </file>
@@ -751,7 +825,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -761,6 +835,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1078,9 +1155,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{654AAEDF-C7D1-4F87-A8A6-CACAA664CB2C}">
   <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="U3" sqref="U3:V9"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1898,8 +1976,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B63CAED-B215-44CA-8867-65B47B1CA3A3}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection sqref="A1:O1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7:K7"/>
+    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="1">
+      <selection activeCell="J4" sqref="J4:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2916,6 +2997,7 @@
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3424,6 +3506,7 @@
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4023,9 +4106,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAE4B4F2-93DF-469E-87F5-6372484E413F}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection sqref="A1:O1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4805,6 +4889,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5308,9 +5393,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E14948D-5C43-4D1C-AD13-A47B8A6652B9}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5739,6 +5825,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -5801,4 +5888,990 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0E32E0-A5BB-462F-9759-F45195EA0A98}">
+  <dimension ref="A1:O30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.140625" style="4"/>
+    <col min="4" max="4" width="14.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="36.5703125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="27.85546875" style="4" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="L2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0</v>
+      </c>
+      <c r="O2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="195" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0</v>
+      </c>
+      <c r="O3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="150" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0</v>
+      </c>
+      <c r="O5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0</v>
+      </c>
+      <c r="O6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="4">
+        <v>4</v>
+      </c>
+      <c r="D7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="L7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0</v>
+      </c>
+      <c r="O7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="4">
+        <v>4</v>
+      </c>
+      <c r="D8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="120" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="4">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3</v>
+      </c>
+      <c r="D10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="L10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0</v>
+      </c>
+      <c r="O10" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C11" s="4">
+        <v>4</v>
+      </c>
+      <c r="D11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="L11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
+      <c r="O11" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="4">
+        <v>2</v>
+      </c>
+      <c r="D12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="L12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
+        <v>0</v>
+      </c>
+      <c r="O12" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="120" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="L13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2</v>
+      </c>
+      <c r="D14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="L14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0</v>
+      </c>
+      <c r="O14" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="4">
+        <v>4</v>
+      </c>
+      <c r="D15" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="L15" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
+      <c r="O15" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1</v>
+      </c>
+      <c r="D16" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="L16" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N16" s="4">
+        <v>0</v>
+      </c>
+      <c r="O16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C17" s="4">
+        <v>3</v>
+      </c>
+      <c r="D17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="L17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0</v>
+      </c>
+      <c r="O17" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="4">
+        <v>3</v>
+      </c>
+      <c r="D18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="L18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N18" s="4">
+        <v>0</v>
+      </c>
+      <c r="O18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="165" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="4">
+        <v>4</v>
+      </c>
+      <c r="D19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="L19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N19" s="4">
+        <v>0</v>
+      </c>
+      <c r="O19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="D30" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Carnomorphs data and functionality
</commit_message>
<xml_diff>
--- a/Data/Cards_and_Tokens.xlsx
+++ b/Data/Cards_and_Tokens.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saku\WebstormProjects\AlienBag\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BAFB65-40AA-4AE0-AC6E-92117A898A9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E3D275-6129-41A2-B169-F404CEBD6799}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="8" xr2:uid="{E69D66DF-7E14-4EE4-A525-8A32B9516520}"/>
-    <workbookView xWindow="28680" yWindow="-4185" windowWidth="15990" windowHeight="24840" activeTab="1" xr2:uid="{99D5B4DA-9CD6-4AED-9D6A-82F7E738FFC0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="9" xr2:uid="{E69D66DF-7E14-4EE4-A525-8A32B9516520}"/>
   </bookViews>
   <sheets>
     <sheet name="Tokens" sheetId="1" r:id="rId1"/>
@@ -21,8 +20,12 @@
     <sheet name="VoidSeeders Event Cards" sheetId="5" r:id="rId5"/>
     <sheet name="Voidseeders Attack Cards" sheetId="6" r:id="rId6"/>
     <sheet name="Voidseeders Panic Cards" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet5" sheetId="8" r:id="rId8"/>
+    <sheet name="VoidSeeder Aliens" sheetId="8" r:id="rId8"/>
     <sheet name="AfterMath Event Deck" sheetId="9" r:id="rId9"/>
+    <sheet name="Carno Tokens" sheetId="11" r:id="rId10"/>
+    <sheet name="Carno Event Cards" sheetId="12" r:id="rId11"/>
+    <sheet name="Carno Attack Cards" sheetId="13" r:id="rId12"/>
+    <sheet name="Carno Aliens" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="319">
   <si>
     <t>ID</t>
   </si>
@@ -790,6 +793,213 @@
   </si>
   <si>
     <t>Speciel Case 5: Alert: Drawn an alert card.</t>
+  </si>
+  <si>
+    <t>Butcher</t>
+  </si>
+  <si>
+    <t>Fleshbeast</t>
+  </si>
+  <si>
+    <t>Shambler</t>
+  </si>
+  <si>
+    <t>Red Metagorger</t>
+  </si>
+  <si>
+    <t>Blue Metagorger</t>
+  </si>
+  <si>
+    <t>Devour</t>
+  </si>
+  <si>
+    <t>If the Character has at least 1 Serious Wound, they die. If not, the Character suffers 1 Serious Wound. The Butcher removes all its Injury Markers.</t>
+  </si>
+  <si>
+    <t>AlienHealthMetagorger</t>
+  </si>
+  <si>
+    <t>Spawn</t>
+  </si>
+  <si>
+    <t>Place a Metagorger miniature in the Room. The Character gets a Slime marker.</t>
+  </si>
+  <si>
+    <t>Bash</t>
+  </si>
+  <si>
+    <t>The Caracter suffers 1 Serious Wound and get 1 Contamination Card.</t>
+  </si>
+  <si>
+    <t>Regurgiate</t>
+  </si>
+  <si>
+    <t>The Character gets a Slime marker and 1 Contamination Card. Place an Intruder Carcass token in the Room.</t>
+  </si>
+  <si>
+    <t>Slash</t>
+  </si>
+  <si>
+    <t>If the Character has 2 Serious Wounds, they die. If not, they suffer 1 Serious Wound.</t>
+  </si>
+  <si>
+    <t>Whiplash</t>
+  </si>
+  <si>
+    <t>The Character suffers 2 Light Wounds and 1 Contamination Card.</t>
+  </si>
+  <si>
+    <t>Rampart Mutation</t>
+  </si>
+  <si>
+    <t>All Characters draw 4 cards from their Action deck and Scan each Contamination card drawn. If there it atleas 1 INFECTED result, the Character gets a Mutation marker. Discard all drawn cards.</t>
+  </si>
+  <si>
+    <t>[3,5]</t>
+  </si>
+  <si>
+    <t>[1,2,5]</t>
+  </si>
+  <si>
+    <t>Reawakening</t>
+  </si>
+  <si>
+    <t>In each Room with a Carcass token (not in a a Character's Hands), replace 1 Carcass token with 1 Shambler. If there is a Character in any of these Rooms, perform 1 Intruder Attack for each Shambler placed that way.</t>
+  </si>
+  <si>
+    <t>[1,2,3,5]</t>
+  </si>
+  <si>
+    <t>Remove from the board all Carnomorphs which are not in a Room with any Character except Metagorgers. Put their respective tokens into the Intruder bag.</t>
+  </si>
+  <si>
+    <t>[1,2,4]</t>
+  </si>
+  <si>
+    <t>Stalking</t>
+  </si>
+  <si>
+    <t>Move all Shamblers, Fleshbeasts and the Butcher to any neighboring Room with a Character, if any. If there are several Rooms possible, move the Carnomorph to the Room with the lowest Number.</t>
+  </si>
+  <si>
+    <t>[1,2,3,4,5]</t>
+  </si>
+  <si>
+    <t>Airlock Procedure Glitch</t>
+  </si>
+  <si>
+    <t>Start the Emergency Airlock Procedure in the Yellow Room with the highest Number.</t>
+  </si>
+  <si>
+    <t>Generator Overload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If there are at least 3 Malfunction markers on the board, start the Self-Destruct Sequence. </t>
+  </si>
+  <si>
+    <t>If there are at least 3 Malfunction markers on the board, start the Self-Destruct Sequence. Remove this card from the game and reshuffle the event deck.</t>
+  </si>
+  <si>
+    <t>Marked Prey</t>
+  </si>
+  <si>
+    <t>All Characters in a Room with a Heavy Object (Intruder Egg, Intruder Carcass or Character Corpse) or carrying such an Object get a Slime marker.</t>
+  </si>
+  <si>
+    <t>Evacuation Hatches Jam</t>
+  </si>
+  <si>
+    <t>Place a Malfunction marker in Evacuation Sections A and B</t>
+  </si>
+  <si>
+    <t>[1,2,3,4]</t>
+  </si>
+  <si>
+    <t>Quarantine Procedure</t>
+  </si>
+  <si>
+    <t>Close all Doors in Corridors connected to Rooms containing each Character with a Slime marker.</t>
+  </si>
+  <si>
+    <t>Growl</t>
+  </si>
+  <si>
+    <t>Place a Noise marker in each Corridor connected to every Room with a Carnomorph.</t>
+  </si>
+  <si>
+    <t>Scavenging Biomatter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move any Carnomorphs (except the Butcher) to any neighboring Rooms with a Heavy Object (Intruder Egg, Intruder Carcass or Character Corpse). Objects in Characters' Hands count. If there are several Rooms possible, move the Carnomorphs to the Room with the lowest Number. </t>
+  </si>
+  <si>
+    <t>Structural Weakness</t>
+  </si>
+  <si>
+    <t>Put a Malfunction marker on each discovered White Room. Remove this card from the game and reshuffle the Event deck.</t>
+  </si>
+  <si>
+    <t>Emergency Protocol Failure</t>
+  </si>
+  <si>
+    <t>Remove the Escape Pod with the highest number from Evacuation Section B, Remove this card from the game and reshuffle the Event deck.</t>
+  </si>
+  <si>
+    <t>Chemical Fire</t>
+  </si>
+  <si>
+    <t>Place a Malfunction marker in the Room with the highest Number containing a Fire marker. Remove that fire marker. Place a Fire marker in all neighboring Rooms. Fire doesn't spread through Technical Corridors or Closed Doors. Reshuffle this card into Event Deck.</t>
+  </si>
+  <si>
+    <t>Ammunition Meltdown</t>
+  </si>
+  <si>
+    <t>Set the item counter to 0 in the Red Room with the lowest Number. Place a Fire marker in this and all neighboring Rooms. Fire doesn't spread through Technical Corridors or Closed Doors. Remove this card from the game and reshuffle the Event deck.</t>
+  </si>
+  <si>
+    <t>[3]</t>
+  </si>
+  <si>
+    <t>Beast on the Prowl</t>
+  </si>
+  <si>
+    <t>If the Butcher is on the board and isn't in a Room with any Character, place it in a room containing a Character with a Slime marker. If several Characters have a Slime marker, choose the first Character in turn order. If the Butcher is not on the board, all Characters with a Slime marker roll for Noise.</t>
+  </si>
+  <si>
+    <t>Remove from the Board all Shamblers which are not in a Room with any Character. Add their tokens to the bag. Add 1 Metagorger to thew Intruder bag. The all players performs a noise roll in order, except if their Character is already in Combat with an Intruder. Return the Blank token to the bag.</t>
+  </si>
+  <si>
+    <t>Remove from the Board all Shamblers which are not in a Room with any Character. Add their tokens to the bag.  The all players performs a noise roll in order, except if their Character is already in Combat with an Intruder.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Place a Noise marker in each Corridor connected to the Room where the Encounter took place. </t>
+  </si>
+  <si>
+    <t>All players perform a Noise roll in order, except if their Character is already in Combat with an Intruder. Remove this token from the Intruder bag and add 1 Metagorger token to the Intruder bag.</t>
+  </si>
+  <si>
+    <t>All players perform a Noise roll in order, except if their Character is already in Combat with an Intruder.</t>
+  </si>
+  <si>
+    <t>Metagorger</t>
+  </si>
+  <si>
+    <t>Place a Metagorger miniature in each Room already containing a Metagorger (even in Combat) and/or a Heavy Object (even if that Object is in a Character's Hands!). If the Nest is explored and not destroyed, also place one Metagorger there. Return the Metagorger token to the bag.</t>
+  </si>
+  <si>
+    <t>Return the Shambler token to the bag. All players perform a Noise roll in order, except if their Character is already in Combat with an Intruder.</t>
+  </si>
+  <si>
+    <t>Return the Fleshbeast token to the bag. All players perform a Noise roll in order, except if their Character is already in Combat with an Intruder.</t>
+  </si>
+  <si>
+    <t>Place the Butcher miniature in a Room containing a Character with a Slime marker and resolve an Encounter. If there are more than one Character with a Slime marker, the one with the fewest cards in hand is affected. In case of tie, use the Character order. If there is no Character with a Slime marker, the Butcher appears in the Room containing the first player. Remove the Butcher token from the bag.</t>
+  </si>
+  <si>
+    <t>Place the Butcher miniature in a Room containing a Character with a Slime marker and resolve an Encounter. If there are more than one Character with a Slime marker, the one with the fewest cards in hand is affected. In case of tie, use the Character order. If there is no Character with a Slime marker, the Butcher appears in the Room containing the first player.</t>
+  </si>
+  <si>
+    <t>Place a Metagorger miniature in each Room already containing a Metagorger (even in Combat) and/or a Heavy Object (even if that Object is in a Character's Hands!). If the Nest is explored and not destroyed, also place one Metagorger there. The metagorgers do not perform surpise attacks.</t>
   </si>
 </sst>
 </file>
@@ -825,7 +1035,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -838,6 +1048,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1155,10 +1371,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{654AAEDF-C7D1-4F87-A8A6-CACAA664CB2C}">
   <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3:V9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29:D30"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1972,15 +2187,2322 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EE07704-C7E6-4A44-8692-A0F66E681331}">
+  <dimension ref="A1:H28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="34" style="3" customWidth="1"/>
+    <col min="6" max="6" width="65.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="46" style="3" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="H2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>253</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>253</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>253</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>253</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>253</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>252</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="H13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>252</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="H14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>252</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="H15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>252</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="H16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>252</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="H17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>252</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="H18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="H19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>252</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="H20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>252</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="H21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>252</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="H22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="H23" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>252</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="H24" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>251</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="H25" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="H26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>251</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="H27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>250</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875439DF-F74F-41E0-A7FF-08AE1AC754AE}">
+  <dimension ref="A1:O21"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection sqref="A1:O1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="55.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="54.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="K12" s="3"/>
+      <c r="L12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="K13" s="3"/>
+      <c r="L13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="2">
+        <v>3</v>
+      </c>
+      <c r="D15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="K15" s="3"/>
+      <c r="L15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="L16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="2">
+        <v>4</v>
+      </c>
+      <c r="D17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="K17" s="3"/>
+      <c r="L17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3</v>
+      </c>
+      <c r="D18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="K19" s="3"/>
+      <c r="L19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M19" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="K20" s="3"/>
+      <c r="L20" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M20" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="N20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C21" s="2">
+        <v>4</v>
+      </c>
+      <c r="D21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="K21" s="3"/>
+      <c r="L21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B89666F7-46F6-45BF-92DB-2419FF29C2F6}">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="3" customWidth="1"/>
+    <col min="2" max="4" width="39.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E2" s="3">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E3" s="3">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="E4" s="3">
+        <v>4</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="E5" s="3">
+        <v>7</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E6" s="3">
+        <v>5</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E8" s="3">
+        <v>5</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E9" s="3">
+        <v>4</v>
+      </c>
+      <c r="F9" s="3">
+        <v>3</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="3">
+        <v>6</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="3">
+        <v>3</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E13" s="3">
+        <v>4</v>
+      </c>
+      <c r="F13" s="3">
+        <v>2</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E14" s="3">
+        <v>5</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E15" s="3">
+        <v>8</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E16" s="3">
+        <v>6</v>
+      </c>
+      <c r="F16" s="3">
+        <v>3</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E17" s="3">
+        <v>7</v>
+      </c>
+      <c r="F17" s="3">
+        <v>3</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E20" s="3">
+        <v>8</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E21" s="3">
+        <v>4</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F486066F-D516-41AD-A6AE-9A9F446EA1D3}">
+  <dimension ref="A4:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>250</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B63CAED-B215-44CA-8867-65B47B1CA3A3}">
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="J7" sqref="J7:K7"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="1">
-      <selection activeCell="J4" sqref="J4:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2997,7 +5519,6 @@
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3504,9 +6025,8 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4109,7 +6629,6 @@
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection sqref="A1:O1"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4889,7 +7408,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5396,7 +7914,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5825,7 +8342,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -5894,10 +8410,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0E32E0-A5BB-462F-9759-F45195EA0A98}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>